<commit_message>
Multi-parameter Cox modeling, PCA and correlation
</commit_message>
<xml_diff>
--- a/data/variable_lexicon.xlsx
+++ b/data/variable_lexicon.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="172">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -509,6 +509,33 @@
   </si>
   <si>
     <t xml:space="preserve">pg/mL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDH_class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lactate dehydrogenase, blood concentration strata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDH strata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AFP_class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpha fetoprotein, blood concentration strata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AFP strata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCG_class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human chorionic gonadotropin, blood concentration strata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCG strata</t>
   </si>
 </sst>
 </file>
@@ -622,13 +649,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.07"/>
@@ -1366,7 +1393,7 @@
         <v>24</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1389,7 +1416,7 @@
         <v>24</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1595,6 +1622,66 @@
         <v>24</v>
       </c>
       <c r="G45" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G48" s="0" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Differences in Figures and Tables
</commit_message>
<xml_diff>
--- a/data/variable_lexicon.xlsx
+++ b/data/variable_lexicon.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="191">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -322,6 +322,24 @@
     <t xml:space="preserve">AFP strata</t>
   </si>
   <si>
+    <t xml:space="preserve">HCG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human chorionic gonadotropin, blood concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IU/L </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCG_class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human chorionic gonadotropin, blood concentration strata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCG strata</t>
+  </si>
+  <si>
     <t xml:space="preserve">LDH</t>
   </si>
   <si>
@@ -340,6 +358,15 @@
     <t xml:space="preserve">LDH strata</t>
   </si>
   <si>
+    <t xml:space="preserve">marker_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AFP and HCG status: negative for both markers or positive for at least one of them</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marker status</t>
+  </si>
+  <si>
     <t xml:space="preserve">surgery_date</t>
   </si>
   <si>
@@ -421,6 +448,9 @@
     <t xml:space="preserve">Total testosterone, blood concentration strata</t>
   </si>
   <si>
+    <t xml:space="preserve">Total testosterone strata</t>
+  </si>
+  <si>
     <t xml:space="preserve">T total strata</t>
   </si>
   <si>
@@ -481,24 +511,6 @@
     <t xml:space="preserve">PRL strata</t>
   </si>
   <si>
-    <t xml:space="preserve">HCG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human chorionic gonadotropin, blood concentration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IU/L </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HCG_class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human chorionic gonadotropin, blood concentration strata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HCG strata</t>
-  </si>
-  <si>
     <t xml:space="preserve">FSH</t>
   </si>
   <si>
@@ -581,15 +593,6 @@
   </si>
   <si>
     <t xml:space="preserve">Date of relapse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marker_status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AFP and HCG status: negative for both markers or positive for at least one of them</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marker status</t>
   </si>
 </sst>
 </file>
@@ -705,11 +708,11 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G55" activeCellId="0" sqref="G55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.07"/>
@@ -1262,7 +1265,7 @@
       <c r="D26" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="2" t="s">
         <v>102</v>
       </c>
       <c r="F26" s="0" t="s">
@@ -1300,56 +1303,59 @@
         <v>107</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>108</v>
-      </c>
       <c r="F28" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>109</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="C29" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>112</v>
-      </c>
       <c r="D29" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>29</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>109</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>114</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>114</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>29</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>109</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1360,67 +1366,67 @@
         <v>116</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="0" t="s">
         <v>118</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>29</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>125</v>
@@ -1429,7 +1435,7 @@
         <v>29</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,96 +1446,90 @@
         <v>127</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>29</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B37" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>96</v>
-      </c>
       <c r="F37" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>138</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>20</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="C39" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>143</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>143</v>
@@ -1538,7 +1538,7 @@
         <v>29</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1549,179 +1549,179 @@
         <v>145</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>96</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>20</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="C41" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="C41" s="0" t="s">
-        <v>147</v>
-      </c>
       <c r="D41" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>20</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>29</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="C43" s="0" t="s">
-        <v>153</v>
-      </c>
       <c r="D43" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>20</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B44" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C44" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="C44" s="0" t="s">
-        <v>158</v>
-      </c>
       <c r="D44" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>159</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>164</v>
-      </c>
       <c r="D46" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>165</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>169</v>
@@ -1729,102 +1729,105 @@
       <c r="D48" s="0" t="s">
         <v>169</v>
       </c>
+      <c r="E48" s="0" t="s">
+        <v>165</v>
+      </c>
       <c r="F48" s="0" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>173</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B50" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="C50" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="D50" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="F50" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="F50" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G50" s="0" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B51" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="C51" s="0" t="s">
         <v>181</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>182</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>182</v>
       </c>
+      <c r="E51" s="0" t="s">
+        <v>183</v>
+      </c>
       <c r="F51" s="0" t="s">
         <v>20</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>186</v>
@@ -1833,33 +1836,32 @@
         <v>186</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>178</v>
+      </c>
+    </row>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>